<commit_message>
Level 36, Submarine optimize, mine particle fix
</commit_message>
<xml_diff>
--- a/Tanks and behaviour.xlsx
+++ b/Tanks and behaviour.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC44109-3C1B-4693-99C0-F7127A0B80CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F67D2F0-D918-42D5-A2C9-11638D146B41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,13 +410,13 @@
     <t>1 * 3 + 11 * 4</t>
   </si>
   <si>
-    <t>New 11 invisible</t>
-  </si>
-  <si>
     <t>New 5 sub</t>
   </si>
   <si>
     <t>7 + 9 + 10 * 2 + 11 * 2 + 15 * x</t>
+  </si>
+  <si>
+    <t>3 * x + 5 * 6</t>
   </si>
 </sst>
 </file>
@@ -906,7 +906,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,6 +1225,9 @@
       <c r="J7" s="10">
         <v>5</v>
       </c>
+      <c r="K7" s="10">
+        <v>36</v>
+      </c>
       <c r="L7" s="15" t="s">
         <v>23</v>
       </c>
@@ -1807,7 +1810,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2168,13 +2171,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>36</v>
       </c>
+      <c r="B37" s="22" t="s">
+        <v>131</v>
+      </c>
       <c r="C37" s="22" t="s">
         <v>129</v>
       </c>
@@ -2187,9 +2193,6 @@
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>38</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Level 37 + mine with mine trigger fixed
</commit_message>
<xml_diff>
--- a/Tanks and behaviour.xlsx
+++ b/Tanks and behaviour.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F67D2F0-D918-42D5-A2C9-11638D146B41}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09812C79-B634-4E2E-8E96-3418E0E1AB0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="133">
   <si>
     <t>Tank color:</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>3 * x + 5 * 6</t>
+  </si>
+  <si>
+    <t>2 + 4 + 11 + 16 + 18 + 20</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1813,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,6 +2192,9 @@
       <c r="A38" s="10">
         <v>37</v>
       </c>
+      <c r="B38" s="22" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10">

</xml_diff>

<commit_message>
Level 38 + laser tank behaviour update
</commit_message>
<xml_diff>
--- a/Tanks and behaviour.xlsx
+++ b/Tanks and behaviour.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09812C79-B634-4E2E-8E96-3418E0E1AB0A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1219310B-8550-4535-933B-C9D1B7808F7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="135">
   <si>
     <t>Tank color:</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>2 + 4 + 11 + 16 + 18 + 20</t>
+  </si>
+  <si>
+    <t>New 8 laser</t>
+  </si>
+  <si>
+    <t>8 * 2 + 9 * 4</t>
   </si>
 </sst>
 </file>
@@ -908,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,6 +1686,9 @@
       <c r="J18" s="10">
         <v>8</v>
       </c>
+      <c r="K18" s="10">
+        <v>38</v>
+      </c>
       <c r="L18" s="15" t="s">
         <v>56</v>
       </c>
@@ -1812,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B488F745-BE2D-4DEE-B3B6-A30AC42C85F0}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,6 +2209,12 @@
       <c r="A39" s="10">
         <v>38</v>
       </c>
+      <c r="B39" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="22" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="10">

</xml_diff>

<commit_message>
Level 43 + telepad fix
</commit_message>
<xml_diff>
--- a/Tanks and behaviour.xlsx
+++ b/Tanks and behaviour.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63B728C-DC9E-4B27-8713-7EBBD8817070}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA224FF-FF01-450C-8CC6-188CC620127F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="147">
   <si>
     <t>Tank color:</t>
   </si>
@@ -459,6 +459,9 @@
   </si>
   <si>
     <t>8 * 2 + 14 * 2</t>
+  </si>
+  <si>
+    <t>3 * x + 10 + 14 + 16</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1858,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,6 +2294,12 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>43</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>146</v>
+      </c>
       <c r="C44" s="22" t="s">
         <v>143</v>
       </c>

</xml_diff>